<commit_message>
tested jb_cp, jb_tr, changed structure & added new module
</commit_message>
<xml_diff>
--- a/RQ1_Res.xlsx
+++ b/RQ1_Res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\Documents\master-thesis\MSThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37586FDB-1D37-4B69-9B02-C8BA3F19D94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CF66A5-CE8E-4C54-B9ED-23300FDC5E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JB_LS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="102">
   <si>
     <t>testcase</t>
   </si>
@@ -204,13 +204,148 @@
   </si>
   <si>
     <t>tc3_2</t>
+  </si>
+  <si>
+    <t>tc22</t>
+  </si>
+  <si>
+    <t>tc23</t>
+  </si>
+  <si>
+    <t>int typed to byte</t>
+  </si>
+  <si>
+    <t>extra stack var in Soot</t>
+  </si>
+  <si>
+    <t>boolean as int in Jimple but type is correct</t>
+  </si>
+  <si>
+    <t>null stmt removed in Soot, in SootUp null var is assigned Obj type</t>
+  </si>
+  <si>
+    <t>b var got removed in both</t>
+  </si>
+  <si>
+    <t>b var got removed in both, int to byte</t>
+  </si>
+  <si>
+    <t>c var got removed in both, int to byte</t>
+  </si>
+  <si>
+    <t>obj of type str instead of obj</t>
+  </si>
+  <si>
+    <t>extra () calls static invoke Integer.valueof, arraylist typed to obj, new #L0, #L1</t>
+  </si>
+  <si>
+    <t>int to byte</t>
+  </si>
+  <si>
+    <t>a cal directly no static call</t>
+  </si>
+  <si>
+    <t>char to byte</t>
+  </si>
+  <si>
+    <t>short to byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 + 1, but not cal </t>
+  </si>
+  <si>
+    <t>val is propagated to sout also</t>
+  </si>
+  <si>
+    <t>sout not propagated</t>
+  </si>
+  <si>
+    <t>only value is propagated, not to sout</t>
+  </si>
+  <si>
+    <t>val is propagated to condition also</t>
+  </si>
+  <si>
+    <t>tc5_1</t>
+  </si>
+  <si>
+    <t>tc5_2</t>
+  </si>
+  <si>
+    <t>tc5_3</t>
+  </si>
+  <si>
+    <t>b not propagated to stack expression</t>
+  </si>
+  <si>
+    <t>b not propagated to sout</t>
+  </si>
+  <si>
+    <t>tc7_1</t>
+  </si>
+  <si>
+    <t>tc7_2</t>
+  </si>
+  <si>
+    <t>b,c not propagated to sout, b not propagated to stack expression</t>
+  </si>
+  <si>
+    <t>cast correctly propagated</t>
+  </si>
+  <si>
+    <t>b correctly propagated to sout</t>
+  </si>
+  <si>
+    <t>null propagated but not to sout</t>
+  </si>
+  <si>
+    <t>both val not propagated to conditon</t>
+  </si>
+  <si>
+    <t>int to long propagated</t>
+  </si>
+  <si>
+    <t>global var not propagated</t>
+  </si>
+  <si>
+    <t>tc13_1</t>
+  </si>
+  <si>
+    <t>stack array also propagated</t>
+  </si>
+  <si>
+    <t>not propagated</t>
+  </si>
+  <si>
+    <t>input file got propagated, in output not propagated</t>
+  </si>
+  <si>
+    <t>tc17_2</t>
+  </si>
+  <si>
+    <t>if expressions then propagated to stack</t>
+  </si>
+  <si>
+    <t>c var left in condition stack5</t>
+  </si>
+  <si>
+    <t>b not propagated in case</t>
+  </si>
+  <si>
+    <t>b not propagated in case, both val not propagated to conditon</t>
+  </si>
+  <si>
+    <t>tc21_1</t>
+  </si>
+  <si>
+    <t>b,d not propagated in case</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +355,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,9 +392,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -542,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,7 +1012,7 @@
       <c r="A25" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
@@ -898,7 +1040,7 @@
       <c r="A27" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="s">
@@ -909,10 +1051,10 @@
       <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
         <v>24</v>
       </c>
     </row>
@@ -970,10 +1112,10 @@
       <c r="A33" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
         <v>24</v>
       </c>
       <c r="D33" t="s">
@@ -984,10 +1126,10 @@
       <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
         <v>24</v>
       </c>
       <c r="D34" t="s">
@@ -998,10 +1140,10 @@
       <c r="A35" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1009,10 +1151,10 @@
       <c r="A36" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1084,12 +1226,436 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0A71C-0C8D-4607-8B6E-74F51903A3B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="71.6328125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1098,22 +1664,324 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEABA7D8-4D45-46B3-848E-5A9094F34FDC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="83.453125" customWidth="1"/>
+  </cols>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1D8C28-615A-4C5F-B29C-3C7866EC8681}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="78.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
applied jb.ese in soot, cp & constprop, filestruc in jb_ls
</commit_message>
<xml_diff>
--- a/RQ1_Res.xlsx
+++ b/RQ1_Res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\Documents\master-thesis\MSThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CF66A5-CE8E-4C54-B9ED-23300FDC5E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33434822-858D-48D2-A042-10BEBF615757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
     <t>null stmt removed in Soot, in SootUp null var is assigned Obj type</t>
   </si>
   <si>
-    <t>b var got removed in both</t>
-  </si>
-  <si>
     <t>b var got removed in both, int to byte</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>b,d not propagated in case</t>
+  </si>
+  <si>
+    <t>b var got removed in both, since in bytecode b var removed</t>
   </si>
 </sst>
 </file>
@@ -392,11 +392,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,7 +1228,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,7 +1262,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1277,7 +1276,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1291,7 +1290,7 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1305,7 +1304,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1319,12 +1318,12 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1335,7 +1334,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1346,16 +1345,16 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
         <v>79</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1369,7 +1368,7 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1383,29 +1382,29 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -1415,11 +1414,11 @@
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1433,7 +1432,7 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1447,7 +1446,7 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1457,7 +1456,7 @@
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1468,11 +1467,11 @@
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1482,18 +1481,18 @@
       <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1504,11 +1503,11 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1518,7 +1517,7 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1533,7 +1532,7 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1544,29 +1543,29 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1577,7 +1576,7 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1588,14 +1587,14 @@
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1607,7 +1606,7 @@
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1618,18 +1617,18 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1640,7 +1639,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1651,7 +1650,7 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1683,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1D8C28-615A-4C5F-B29C-3C7866EC8681}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1797,10 +1796,10 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1808,7 +1807,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1821,7 +1820,7 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1829,7 +1828,7 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -1872,11 +1871,11 @@
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1886,11 +1885,11 @@
       <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1903,7 +1902,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1917,7 +1916,7 @@
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1927,11 +1926,11 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1950,7 +1949,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
tested jb.uce, jb.ule by compiler
</commit_message>
<xml_diff>
--- a/RQ1_Res.xlsx
+++ b/RQ1_Res.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\Documents\master-thesis\MSThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B28876A-09E5-41A5-9D9B-BA42EC30F6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD95739B-7271-439A-BE6C-5B50897EB7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JB_LS" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="JB_CP" sheetId="7" r:id="rId7"/>
     <sheet name="JB_UCE" sheetId="8" r:id="rId8"/>
     <sheet name="JB_TR" sheetId="9" r:id="rId9"/>
+    <sheet name="JB_LNS" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="137">
   <si>
     <t>testcase</t>
   </si>
@@ -357,6 +358,93 @@
   </si>
   <si>
     <t>switch break applied correctly, labels get rearragned wrongly</t>
+  </si>
+  <si>
+    <t>why y=x got deleted?</t>
+  </si>
+  <si>
+    <t>why x=5, x=60 not removed?</t>
+  </si>
+  <si>
+    <t>tc24</t>
+  </si>
+  <si>
+    <t>tc25</t>
+  </si>
+  <si>
+    <t>tc26</t>
+  </si>
+  <si>
+    <t>tc27</t>
+  </si>
+  <si>
+    <t>x=10 not removed</t>
+  </si>
+  <si>
+    <t>why x=10, x=20 if we sout then not removed</t>
+  </si>
+  <si>
+    <t>x=sm() removed in soot</t>
+  </si>
+  <si>
+    <t>x=5 not removed, y=sm() removed in soot</t>
+  </si>
+  <si>
+    <t>why x=20 not removed, x=sm() removed in soot</t>
+  </si>
+  <si>
+    <t>x=10 not removed, z=sm() removed in soot</t>
+  </si>
+  <si>
+    <t>diff jimple in finally case</t>
+  </si>
+  <si>
+    <t>Soot DAE also removes Nop stmts</t>
+  </si>
+  <si>
+    <t>arr[] ref no effects</t>
+  </si>
+  <si>
+    <t>flag=0 not removed</t>
+  </si>
+  <si>
+    <t>x=15 not removed</t>
+  </si>
+  <si>
+    <t>SootUp invoke func not removed like int x = sm()</t>
+  </si>
+  <si>
+    <t>i++ not removd</t>
+  </si>
+  <si>
+    <t>tc12_1</t>
+  </si>
+  <si>
+    <t>i++ removed</t>
+  </si>
+  <si>
+    <t>i=5 not removed</t>
+  </si>
+  <si>
+    <t>flag=0 not removed, temp = 10 removed in soot</t>
+  </si>
+  <si>
+    <t>Java Compiler itself removes unused local var</t>
+  </si>
+  <si>
+    <t>Nop eliminator in SootUp can't be generated via java source code</t>
+  </si>
+  <si>
+    <t>tc28</t>
+  </si>
+  <si>
+    <t>tc29</t>
+  </si>
+  <si>
+    <t>tc30</t>
+  </si>
+  <si>
+    <t>Doesn't remove from source code</t>
   </si>
 </sst>
 </file>
@@ -410,11 +498,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,6 +787,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1182,11 +1272,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C60968-C8EF-4B05-A358-05624D374EE3}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B75705-77D5-4135-BC36-BC72BB916C48}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
@@ -1194,12 +1286,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C60968-C8EF-4B05-A358-05624D374EE3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="56.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831437A3-0FE3-41D4-BAC3-857A168DAE24}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,7 +1612,7 @@
       <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1491,7 +1623,7 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1502,7 +1634,7 @@
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1513,7 +1645,7 @@
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1525,46 +1657,556 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E79297C-28E4-4FA7-B2C6-7EA3BE6F92F8}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="58" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE2D155-8980-48ED-9F7D-0F3850F6F73E}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="61.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24217E59-62E7-4316-AA4A-CC081F82175C}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="61.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0A71C-0C8D-4607-8B6E-74F51903A3B1}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1997,17 +2639,40 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEABA7D8-4D45-46B3-848E-5A9094F34FDC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="83.453125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2016,10 +2681,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1D8C28-615A-4C5F-B29C-3C7866EC8681}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
sootup getClasses func changed, tc24 25 cp bug, testing cbf
</commit_message>
<xml_diff>
--- a/RQ1_Res.xlsx
+++ b/RQ1_Res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\Documents\master-thesis\MSThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3468995-F7F1-48CA-BA07-9DD6C7D8618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD6E21-71DD-4A91-BCC1-A75A809D640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11860" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JB_LS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="146">
   <si>
     <t>testcase</t>
   </si>
@@ -464,13 +464,22 @@
   </si>
   <si>
     <t>wrong jimple order??</t>
+  </si>
+  <si>
+    <t>cbf perform dead code eliminator at the last step</t>
+  </si>
+  <si>
+    <t>not printed in parameters</t>
+  </si>
+  <si>
+    <t>Bug, should not propagate inside array index, even in Soot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +495,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -517,10 +533,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01127D9B-9278-4A7A-A675-0A71F0BBC6C7}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1709,7 +1727,7 @@
     <col min="4" max="4" width="51.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1722,8 +1740,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1734,72 +1755,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2777,10 +2798,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3202,7 +3223,7 @@
       <c r="D33" t="s">
         <v>100</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3215,6 +3236,62 @@
       </c>
       <c r="D34" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 4 jars, convertcommatosemicolon,rq2
</commit_message>
<xml_diff>
--- a/RQ1_Res.xlsx
+++ b/RQ1_Res.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\Documents\master-thesis\MSThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD6E21-71DD-4A91-BCC1-A75A809D640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8F7619-24EF-4669-A7FC-8E20E38490CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JB_LS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="147">
   <si>
     <t>testcase</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Bug, should not propagate inside array index, even in Soot</t>
+  </si>
+  <si>
+    <t>nested cbf was not working earlier</t>
   </si>
 </sst>
 </file>
@@ -533,12 +536,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,7 +831,7 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1718,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01127D9B-9278-4A7A-A675-0A71F0BBC6C7}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1759,120 +1761,267 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1883,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C60968-C8EF-4B05-A358-05624D374EE3}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1912,8 +2061,213 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2800,7 +3154,7 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -3258,7 +3612,7 @@
       <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3266,7 +3620,7 @@
       <c r="A38" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3274,7 +3628,7 @@
       <c r="A39" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3282,7 +3636,7 @@
       <c r="A40" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3290,7 +3644,7 @@
       <c r="A41" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>